<commit_message>
R file function created for: write column headers and add technical replicates based on plate map.
Function to be written to R file - normalise using plate map.
</commit_message>
<xml_diff>
--- a/Validation/validation_output/example_generated_platemap_manual_changes.xlsx
+++ b/Validation/validation_output/example_generated_platemap_manual_changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\Dropbox (Cambridge University)\NormaliseForIC50\Validation\validation_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97971512-9757-4CB7-AF21-9589FBE9F9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F71C0C-1C9A-462A-83B5-37A75F75DC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4590" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="100">
   <si>
     <t>Plate_Name</t>
   </si>
@@ -300,6 +300,39 @@
   </si>
   <si>
     <t>inhibition</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -321,6 +354,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -709,11 +743,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M125"/>
+  <dimension ref="A1:N125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +756,7 @@
     <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -762,8 +796,11 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -800,8 +837,11 @@
       <c r="M2" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -838,8 +878,11 @@
       <c r="M3" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -876,8 +919,11 @@
       <c r="M4" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -914,8 +960,11 @@
       <c r="M5" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -952,8 +1001,11 @@
       <c r="M6" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -990,8 +1042,11 @@
       <c r="M7" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -1028,8 +1083,11 @@
       <c r="M8" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1066,8 +1124,11 @@
       <c r="M9" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1104,8 +1165,11 @@
       <c r="M10" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1142,8 +1206,11 @@
       <c r="M11" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -1180,8 +1247,11 @@
       <c r="M12" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1218,8 +1288,11 @@
       <c r="M13" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1256,8 +1329,11 @@
       <c r="M14" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -1294,8 +1370,11 @@
       <c r="M15" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -1332,8 +1411,11 @@
       <c r="M16" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -1370,8 +1452,11 @@
       <c r="M17" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -1408,8 +1493,11 @@
       <c r="M18" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -1446,8 +1534,11 @@
       <c r="M19" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -1484,8 +1575,11 @@
       <c r="M20" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -1522,8 +1616,11 @@
       <c r="M21" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -1560,8 +1657,11 @@
       <c r="M22" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -1598,8 +1698,11 @@
       <c r="M23" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -1636,8 +1739,11 @@
       <c r="M24" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -1674,8 +1780,11 @@
       <c r="M25" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -1712,8 +1821,11 @@
       <c r="M26" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -1750,8 +1862,11 @@
       <c r="M27" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -1788,8 +1903,11 @@
       <c r="M28" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -1826,8 +1944,11 @@
       <c r="M29" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1864,8 +1985,11 @@
       <c r="M30" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -1902,8 +2026,11 @@
       <c r="M31" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -1940,8 +2067,11 @@
       <c r="M32" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -1978,8 +2108,11 @@
       <c r="M33" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>87</v>
       </c>
@@ -2016,8 +2149,11 @@
       <c r="M34" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>87</v>
       </c>
@@ -2054,8 +2190,11 @@
       <c r="M35" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -2092,8 +2231,11 @@
       <c r="M36" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -2130,8 +2272,11 @@
       <c r="M37" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -2168,8 +2313,11 @@
       <c r="M38" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -2206,8 +2354,11 @@
       <c r="M39" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2244,8 +2395,11 @@
       <c r="M40" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -2282,8 +2436,11 @@
       <c r="M41" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -2320,8 +2477,11 @@
       <c r="M42" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -2358,8 +2518,11 @@
       <c r="M43" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -2396,8 +2559,11 @@
       <c r="M44" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -2434,8 +2600,11 @@
       <c r="M45" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -2472,8 +2641,11 @@
       <c r="M46" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -2510,8 +2682,11 @@
       <c r="M47" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -2548,8 +2723,11 @@
       <c r="M48" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -2586,8 +2764,11 @@
       <c r="M49" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -2624,8 +2805,11 @@
       <c r="M50" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>87</v>
       </c>
@@ -2662,8 +2846,11 @@
       <c r="M51" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -2700,8 +2887,11 @@
       <c r="M52" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -2738,8 +2928,11 @@
       <c r="M53" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>87</v>
       </c>
@@ -2776,8 +2969,11 @@
       <c r="M54" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -2814,8 +3010,11 @@
       <c r="M55" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -2852,8 +3051,11 @@
       <c r="M56" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -2890,8 +3092,11 @@
       <c r="M57" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>87</v>
       </c>
@@ -2928,8 +3133,11 @@
       <c r="M58" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>87</v>
       </c>
@@ -2966,8 +3174,11 @@
       <c r="M59" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -3004,8 +3215,11 @@
       <c r="M60" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>87</v>
       </c>
@@ -3042,8 +3256,11 @@
       <c r="M61" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -3080,8 +3297,11 @@
       <c r="M62" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>87</v>
       </c>
@@ -3118,8 +3338,11 @@
       <c r="M63" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>87</v>
       </c>
@@ -3156,8 +3379,11 @@
       <c r="M64" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>87</v>
       </c>
@@ -3194,8 +3420,11 @@
       <c r="M65" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -3232,8 +3461,11 @@
       <c r="M66" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N66" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>87</v>
       </c>
@@ -3270,8 +3502,11 @@
       <c r="M67" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -3308,8 +3543,11 @@
       <c r="M68" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>87</v>
       </c>
@@ -3346,8 +3584,11 @@
       <c r="M69" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N69" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -3384,8 +3625,11 @@
       <c r="M70" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N70" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>87</v>
       </c>
@@ -3422,8 +3666,11 @@
       <c r="M71" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -3460,8 +3707,11 @@
       <c r="M72" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N72" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -3498,8 +3748,11 @@
       <c r="M73" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N73" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -3536,8 +3789,11 @@
       <c r="M74" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N74" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -3574,8 +3830,11 @@
       <c r="M75" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N75" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -3612,8 +3871,11 @@
       <c r="M76" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N76" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -3650,8 +3912,11 @@
       <c r="M77" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -3688,8 +3953,11 @@
       <c r="M78" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N78" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -3726,8 +3994,11 @@
       <c r="M79" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N79" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -3764,8 +4035,11 @@
       <c r="M80" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N80" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -3802,8 +4076,11 @@
       <c r="M81" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -3840,8 +4117,11 @@
       <c r="M82" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N82" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -3878,8 +4158,11 @@
       <c r="M83" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N83" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -3916,8 +4199,11 @@
       <c r="M84" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N84" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -3954,8 +4240,11 @@
       <c r="M85" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N85" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -3992,8 +4281,11 @@
       <c r="M86" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N86" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -4030,8 +4322,11 @@
       <c r="M87" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N87" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -4068,8 +4363,11 @@
       <c r="M88" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N88" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -4106,8 +4404,11 @@
       <c r="M89" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N89" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>87</v>
       </c>
@@ -4144,8 +4445,11 @@
       <c r="M90" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N90" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -4182,8 +4486,11 @@
       <c r="M91" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N91" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -4220,8 +4527,11 @@
       <c r="M92" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>87</v>
       </c>
@@ -4258,8 +4568,11 @@
       <c r="M93" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N93" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>87</v>
       </c>
@@ -4296,8 +4609,11 @@
       <c r="M94" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N94" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>87</v>
       </c>
@@ -4334,8 +4650,11 @@
       <c r="M95" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N95" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>87</v>
       </c>
@@ -4372,8 +4691,11 @@
       <c r="M96" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N96" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>87</v>
       </c>
@@ -4410,8 +4732,11 @@
       <c r="M97" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N97" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>87</v>
       </c>
@@ -4448,8 +4773,11 @@
       <c r="M98" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N98" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -4486,8 +4814,11 @@
       <c r="M99" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N99" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>87</v>
       </c>
@@ -4524,8 +4855,11 @@
       <c r="M100" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N100" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>87</v>
       </c>
@@ -4562,8 +4896,11 @@
       <c r="M101" s="1">
         <v>44808</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N101" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>88</v>
       </c>
@@ -4600,8 +4937,11 @@
       <c r="M102" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N102" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>88</v>
       </c>
@@ -4638,8 +4978,11 @@
       <c r="M103" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N103" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>88</v>
       </c>
@@ -4676,8 +5019,11 @@
       <c r="M104" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N104" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>88</v>
       </c>
@@ -4714,8 +5060,11 @@
       <c r="M105" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N105" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>88</v>
       </c>
@@ -4752,8 +5101,11 @@
       <c r="M106" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N106" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>88</v>
       </c>
@@ -4790,8 +5142,11 @@
       <c r="M107" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N107" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>88</v>
       </c>
@@ -4828,8 +5183,11 @@
       <c r="M108" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N108" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>88</v>
       </c>
@@ -4866,8 +5224,11 @@
       <c r="M109" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N109" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>88</v>
       </c>
@@ -4904,8 +5265,11 @@
       <c r="M110" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N110" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>88</v>
       </c>
@@ -4942,8 +5306,11 @@
       <c r="M111" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N111" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>88</v>
       </c>
@@ -4980,8 +5347,11 @@
       <c r="M112" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N112" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>88</v>
       </c>
@@ -5018,8 +5388,11 @@
       <c r="M113" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N113" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>88</v>
       </c>
@@ -5056,8 +5429,11 @@
       <c r="M114" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N114" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>88</v>
       </c>
@@ -5094,8 +5470,11 @@
       <c r="M115" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N115" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>88</v>
       </c>
@@ -5132,8 +5511,11 @@
       <c r="M116" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N116" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>88</v>
       </c>
@@ -5170,8 +5552,11 @@
       <c r="M117" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N117" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>88</v>
       </c>
@@ -5208,8 +5593,11 @@
       <c r="M118" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N118" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>88</v>
       </c>
@@ -5246,8 +5634,11 @@
       <c r="M119" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N119" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>88</v>
       </c>
@@ -5284,8 +5675,11 @@
       <c r="M120" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N120" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>88</v>
       </c>
@@ -5322,8 +5716,11 @@
       <c r="M121" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N121" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>88</v>
       </c>
@@ -5360,8 +5757,11 @@
       <c r="M122" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N122" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -5398,8 +5798,11 @@
       <c r="M123" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N123" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>88</v>
       </c>
@@ -5436,8 +5839,11 @@
       <c r="M124" s="1">
         <v>45367</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N124" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>88</v>
       </c>
@@ -5473,6 +5879,9 @@
       </c>
       <c r="M125" s="1">
         <v>45367</v>
+      </c>
+      <c r="N125" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>